<commit_message>
Add new H2 turbine
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-turbine.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-turbine.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3999D57-E14F-2A45-AA06-99682CB0BA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A380463-7CE2-DD46-87F5-D3B646E5BF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{26241F67-8618-094B-AD38-E491C9570B84}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{26241F67-8618-094B-AD38-E491C9570B84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="58">
   <si>
     <t>database</t>
   </si>
@@ -128,9 +128,6 @@
     <t>H2-fed 1 GW gas turbine used for grid-balancing. Use a CCGT dataset for infrastructure. Capacity: 1000 MW. Capacity factor: 70%. Efficiency (HHV): 51.3%. Yearly production: 6,004,454 MWh.</t>
   </si>
   <si>
-    <t>electricity production, from hydrogen-fired one gigawatt gas turbine</t>
-  </si>
-  <si>
     <t>gas power plant construction, combined cycle, 400MW electrical</t>
   </si>
   <si>
@@ -201,6 +198,21 @@
   </si>
   <si>
     <t>Assumes 95% LHV efficiency + 0.5% H2 loss</t>
+  </si>
+  <si>
+    <t>heat production, from hydrogen-fired one gigawatt gas turbine, for grid balancing</t>
+  </si>
+  <si>
+    <t>electricity production, from hydrogen-fired one gigawatt gas turbine, for grid balancing</t>
+  </si>
+  <si>
+    <t>market for hydrogen, gaseous, low pressure</t>
+  </si>
+  <si>
+    <t>hydrogen, gaseous, low pressure</t>
+  </si>
+  <si>
+    <t>H2-fed 1 GW hydrogen gas turbine. Use a CCGT dataset for infrastructure. Capacity: 1000 MW. Capacity factor: 70%. Efficiency (HHV): 95%. Yearly production: 6,004,454 MWh.</t>
   </si>
 </sst>
 </file>
@@ -574,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1C5B3A-29A3-3D4D-87B5-E2283E6AD55F}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -603,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="M3" t="s">
         <v>2</v>
@@ -717,7 +729,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>B3</f>
-        <v>electricity production, from hydrogen-fired one gigawatt gas turbine</v>
+        <v>electricity production, from hydrogen-fired one gigawatt gas turbine, for grid balancing</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -740,7 +752,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3">
         <v>1.3888999999999999E-11</v>
@@ -755,12 +767,12 @@
         <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3">
         <f>((3.6/0.513)/141.8)*1.005</f>
@@ -776,10 +788,10 @@
         <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -794,18 +806,18 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3">
         <v>1.5428571428571401E-4</v>
@@ -814,18 +826,18 @@
         <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="4">
         <f>((3.6/0.513)/141.8)*0.005</f>
@@ -841,7 +853,7 @@
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -849,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="M20" t="s">
         <v>2</v>
@@ -898,7 +910,7 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M25" t="s">
         <v>2</v>
@@ -920,7 +932,7 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M27" t="s">
         <v>2</v>
@@ -963,7 +975,7 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>B20</f>
-        <v>heat production, from hydrogen-fired one gigawatt gas turbine</v>
+        <v>heat production, from hydrogen-fired one gigawatt gas turbine, for grid balancing</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -986,7 +998,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="3">
         <f>0.000000000013889/3.6</f>
@@ -1002,16 +1014,16 @@
         <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3">
-        <f>1/120/0.95</f>
-        <v>8.771929824561403E-3</v>
+        <f>(1/120/0.95)*1.02</f>
+        <v>8.9473684210526309E-3</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1023,10 +1035,10 @@
         <v>16</v>
       </c>
       <c r="G32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -1034,25 +1046,25 @@
         <v>21</v>
       </c>
       <c r="B33" s="3">
-        <f>0.4448/1000/3.6</f>
-        <v>1.2355555555555554E-4</v>
+        <f>B32*9/1000</f>
+        <v>8.052631578947368E-5</v>
       </c>
       <c r="D33" t="s">
         <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F33" t="s">
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="3">
         <f>0.000154285714285714/3.6</f>
@@ -1062,22 +1074,22 @@
         <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
       </c>
       <c r="H34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
-        <f>((1/0.513)/141.8)*0.005</f>
-        <v>6.8734758067398537E-5</v>
+        <f>B32*0.02</f>
+        <v>1.7894736842105261E-4</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
@@ -1089,7 +1101,7 @@
         <v>20</v>
       </c>
       <c r="H35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -1097,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="M37" t="s">
         <v>2</v>
@@ -1130,7 +1142,7 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -1138,7 +1150,7 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -1146,7 +1158,7 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M42" t="s">
         <v>2</v>
@@ -1168,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M44" t="s">
         <v>2</v>
@@ -1211,7 +1223,7 @@
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
         <f>B37</f>
-        <v>hydrogen storage, for grid-balancing</v>
+        <v>heat production, from hydrogen-fired one gigawatt gas turbine</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1222,103 +1234,351 @@
       </c>
       <c r="D47" s="2" t="str">
         <f>B44</f>
-        <v>kilogram</v>
+        <v>megajoule</v>
       </c>
       <c r="F47" t="s">
         <v>18</v>
       </c>
       <c r="G47" t="str">
         <f>B42</f>
-        <v>hydrogen, gaseous, 80 bar</v>
+        <v>heat</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" s="4">
+        <v>29</v>
+      </c>
+      <c r="B48" s="3">
+        <f>0.000000000013889/3.6</f>
+        <v>3.8580555555555555E-12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="3">
+        <f>(1/120/0.95)*1.02</f>
+        <v>8.9473684210526309E-3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
+        <v>56</v>
+      </c>
+      <c r="H49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="3">
+        <f>B49*9/1000</f>
+        <v>8.052631578947368E-5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="3">
+        <f>0.000154285714285714/3.6</f>
+        <v>4.2857142857142782E-5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>36</v>
+      </c>
+      <c r="F51" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="4">
+        <f>B49*0.02</f>
+        <v>1.7894736842105261E-4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="M55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="M56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>46</v>
+      </c>
+      <c r="M59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="M60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="M61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" t="str">
+        <f>B54</f>
+        <v>hydrogen storage, for grid-balancing</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="str">
+        <f>B55</f>
+        <v>RER</v>
+      </c>
+      <c r="D64" s="2" t="str">
+        <f>B61</f>
+        <v>kilogram</v>
+      </c>
+      <c r="F64" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" t="str">
+        <f>B59</f>
+        <v>hydrogen, gaseous, 80 bar</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="4">
         <f>1+0.0025+(0.023*0.3)</f>
         <v>1.0093999999999999</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C65" t="s">
         <v>4</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D65" t="s">
         <v>17</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F65" t="s">
         <v>16</v>
       </c>
-      <c r="G48" t="s">
-        <v>33</v>
-      </c>
-      <c r="H48" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="G65" t="s">
+        <v>32</v>
+      </c>
+      <c r="H65" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" s="4">
+        <f>B65</f>
+        <v>1.0093999999999999</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="4">
-        <f>B48</f>
-        <v>1.0093999999999999</v>
-      </c>
-      <c r="C49" t="s">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67">
+        <v>0.88</v>
+      </c>
+      <c r="C67" t="s">
         <v>4</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D67" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" t="s">
+        <v>16</v>
+      </c>
+      <c r="G67" t="s">
+        <v>24</v>
+      </c>
+      <c r="H67" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="4">
+        <f>B66-1</f>
+        <v>9.3999999999998529E-3</v>
+      </c>
+      <c r="D68" t="s">
         <v>17</v>
       </c>
-      <c r="F49" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50">
-        <v>0.88</v>
-      </c>
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>22</v>
-      </c>
-      <c r="F50" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" t="s">
-        <v>24</v>
-      </c>
-      <c r="H50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="E68" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" t="s">
         <v>44</v>
-      </c>
-      <c r="B51" s="4">
-        <f>B49-1</f>
-        <v>9.3999999999998529E-3</v>
-      </c>
-      <c r="D51" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H51" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>